<commit_message>
Added check to catch overflowing data
</commit_message>
<xml_diff>
--- a/Resources/InvoiceASAP_Template_2025_NonTaxable.xlsx
+++ b/Resources/InvoiceASAP_Template_2025_NonTaxable.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaroslavkravchuk/Downloads/MISC/code/tax/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yaroslavkravchuk/Downloads/MISC/code/tax/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D606B5F-1EAB-1445-BF90-7138EF8E2F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7A9962-F9BE-1945-9D0D-F3A3C384B942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20140" tabRatio="689" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -410,6 +410,45 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -418,45 +457,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -828,7 +828,7 @@
   <dimension ref="A1:M73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H68" sqref="A1:H68"/>
+      <selection activeCell="M68" sqref="M68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -848,16 +848,16 @@
     <row r="1" spans="1:13" ht="83.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="16"/>
       <c r="B1" s="16"/>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="36" t="s">
+      <c r="D1" s="39"/>
+      <c r="E1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
       <c r="I1" s="30"/>
       <c r="J1" s="2"/>
       <c r="K1" s="11"/>
@@ -869,10 +869,10 @@
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="15"/>
-      <c r="E2" s="43" t="s">
+      <c r="E2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="43"/>
+      <c r="F2" s="40"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="5"/>
@@ -896,11 +896,11 @@
       <c r="C4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
       <c r="I4" s="5"/>
       <c r="J4" s="2"/>
     </row>
@@ -910,11 +910,11 @@
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
       <c r="I5" s="5"/>
       <c r="J5" s="2"/>
     </row>
@@ -937,17 +937,17 @@
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="39" t="s">
+      <c r="C7" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="40"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="39" t="s">
+      <c r="F7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="40"/>
+      <c r="G7" s="44"/>
       <c r="H7" s="22" t="s">
         <v>11</v>
       </c>
@@ -957,736 +957,736 @@
     <row r="8" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13"/>
       <c r="B8" s="13"/>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
       <c r="E8" s="19"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="38"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="46"/>
       <c r="H8" s="8"/>
-      <c r="I8" s="41"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="47"/>
+      <c r="C9" s="34"/>
+      <c r="D9" s="35"/>
       <c r="E9" s="19"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="38"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="46"/>
       <c r="H9" s="8"/>
-      <c r="I9" s="41"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="47"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="35"/>
       <c r="E10" s="19"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="38"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="46"/>
       <c r="H10" s="8"/>
-      <c r="I10" s="41"/>
+      <c r="I10" s="38"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
       <c r="E11" s="19"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="38"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
       <c r="H11" s="8"/>
-      <c r="I11" s="41"/>
+      <c r="I11" s="38"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="35"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="38"/>
+      <c r="F12" s="45"/>
+      <c r="G12" s="46"/>
       <c r="H12" s="8"/>
-      <c r="I12" s="41"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="47"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="35"/>
       <c r="E13" s="19"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="38"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="46"/>
       <c r="H13" s="8"/>
-      <c r="I13" s="41"/>
+      <c r="I13" s="38"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="35"/>
       <c r="E14" s="19"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="38"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="46"/>
       <c r="H14" s="8"/>
-      <c r="I14" s="41"/>
+      <c r="I14" s="38"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="35"/>
       <c r="E15" s="19"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="38"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="46"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="41"/>
+      <c r="I15" s="38"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13"/>
       <c r="B16" s="13"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="35"/>
       <c r="E16" s="19"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="38"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="46"/>
       <c r="H16" s="8"/>
-      <c r="I16" s="41"/>
+      <c r="I16" s="38"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13"/>
       <c r="B17" s="13"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="35"/>
       <c r="E17" s="19"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="38"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="46"/>
       <c r="H17" s="8"/>
-      <c r="I17" s="41"/>
+      <c r="I17" s="38"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13"/>
       <c r="B18" s="13"/>
-      <c r="C18" s="46"/>
-      <c r="D18" s="47"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="35"/>
       <c r="E18" s="19"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="38"/>
+      <c r="F18" s="45"/>
+      <c r="G18" s="46"/>
       <c r="H18" s="8"/>
-      <c r="I18" s="41"/>
+      <c r="I18" s="38"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13"/>
       <c r="B19" s="13"/>
-      <c r="C19" s="46"/>
-      <c r="D19" s="47"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="19"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="38"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="46"/>
       <c r="H19" s="8"/>
-      <c r="I19" s="41"/>
+      <c r="I19" s="38"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
-      <c r="C20" s="46"/>
-      <c r="D20" s="47"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
       <c r="E20" s="19"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="38"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="46"/>
       <c r="H20" s="8"/>
-      <c r="I20" s="41"/>
+      <c r="I20" s="38"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="47"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="35"/>
       <c r="E21" s="19"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="38"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="46"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="41"/>
+      <c r="I21" s="38"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
-      <c r="C22" s="46"/>
-      <c r="D22" s="47"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="35"/>
       <c r="E22" s="19"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="38"/>
+      <c r="F22" s="45"/>
+      <c r="G22" s="46"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="41"/>
+      <c r="I22" s="38"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="47"/>
+      <c r="C23" s="34"/>
+      <c r="D23" s="35"/>
       <c r="E23" s="19"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="38"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="46"/>
       <c r="H23" s="8"/>
-      <c r="I23" s="41"/>
+      <c r="I23" s="38"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="47"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="35"/>
       <c r="E24" s="19"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="38"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="46"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="41"/>
+      <c r="I24" s="38"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
-      <c r="C25" s="46"/>
-      <c r="D25" s="47"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="35"/>
       <c r="E25" s="19"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="38"/>
+      <c r="F25" s="45"/>
+      <c r="G25" s="46"/>
       <c r="H25" s="8"/>
-      <c r="I25" s="41"/>
+      <c r="I25" s="38"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
-      <c r="C26" s="46"/>
-      <c r="D26" s="47"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="35"/>
       <c r="E26" s="19"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="38"/>
+      <c r="F26" s="45"/>
+      <c r="G26" s="46"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="41"/>
+      <c r="I26" s="38"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="47"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="35"/>
       <c r="E27" s="19"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="38"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="46"/>
       <c r="H27" s="8"/>
-      <c r="I27" s="41"/>
+      <c r="I27" s="38"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
-      <c r="C28" s="46"/>
-      <c r="D28" s="47"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="35"/>
       <c r="E28" s="19"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="38"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="46"/>
       <c r="H28" s="8"/>
-      <c r="I28" s="41"/>
+      <c r="I28" s="38"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="47"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="35"/>
       <c r="E29" s="19"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="38"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="46"/>
       <c r="H29" s="8"/>
-      <c r="I29" s="41"/>
+      <c r="I29" s="38"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="47"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="35"/>
       <c r="E30" s="19"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="38"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="46"/>
       <c r="H30" s="8"/>
-      <c r="I30" s="41"/>
+      <c r="I30" s="38"/>
       <c r="J30" s="1"/>
     </row>
     <row r="31" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
-      <c r="C31" s="46"/>
-      <c r="D31" s="47"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="35"/>
       <c r="E31" s="19"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="38"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="46"/>
       <c r="H31" s="8"/>
-      <c r="I31" s="41"/>
+      <c r="I31" s="38"/>
       <c r="J31" s="1"/>
     </row>
     <row r="32" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
-      <c r="C32" s="46"/>
-      <c r="D32" s="47"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="35"/>
       <c r="E32" s="19"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="38"/>
+      <c r="F32" s="45"/>
+      <c r="G32" s="46"/>
       <c r="H32" s="8"/>
-      <c r="I32" s="41"/>
+      <c r="I32" s="38"/>
       <c r="J32" s="1"/>
     </row>
     <row r="33" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
-      <c r="C33" s="46"/>
-      <c r="D33" s="47"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="35"/>
       <c r="E33" s="19"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="38"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="46"/>
       <c r="H33" s="8"/>
-      <c r="I33" s="41"/>
+      <c r="I33" s="38"/>
       <c r="J33" s="1"/>
     </row>
     <row r="34" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
-      <c r="C34" s="46"/>
-      <c r="D34" s="47"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="35"/>
       <c r="E34" s="19"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="38"/>
+      <c r="F34" s="45"/>
+      <c r="G34" s="46"/>
       <c r="H34" s="8"/>
-      <c r="I34" s="41"/>
+      <c r="I34" s="38"/>
       <c r="J34" s="1"/>
     </row>
     <row r="35" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
-      <c r="C35" s="46"/>
-      <c r="D35" s="47"/>
+      <c r="C35" s="34"/>
+      <c r="D35" s="35"/>
       <c r="E35" s="19"/>
-      <c r="F35" s="37"/>
-      <c r="G35" s="38"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="46"/>
       <c r="H35" s="8"/>
-      <c r="I35" s="41"/>
+      <c r="I35" s="38"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
-      <c r="C36" s="46"/>
-      <c r="D36" s="47"/>
+      <c r="C36" s="34"/>
+      <c r="D36" s="35"/>
       <c r="E36" s="19"/>
-      <c r="F36" s="37"/>
-      <c r="G36" s="38"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="46"/>
       <c r="H36" s="8"/>
-      <c r="I36" s="41"/>
+      <c r="I36" s="38"/>
       <c r="J36" s="1"/>
     </row>
     <row r="37" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
-      <c r="C37" s="46"/>
-      <c r="D37" s="47"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="35"/>
       <c r="E37" s="19"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="38"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="46"/>
       <c r="H37" s="8"/>
-      <c r="I37" s="41"/>
+      <c r="I37" s="38"/>
       <c r="J37" s="1"/>
     </row>
     <row r="38" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
-      <c r="C38" s="46"/>
-      <c r="D38" s="47"/>
+      <c r="C38" s="34"/>
+      <c r="D38" s="35"/>
       <c r="E38" s="19"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="38"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="46"/>
       <c r="H38" s="8"/>
-      <c r="I38" s="41"/>
+      <c r="I38" s="38"/>
       <c r="J38" s="1"/>
     </row>
     <row r="39" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="47"/>
+      <c r="C39" s="34"/>
+      <c r="D39" s="35"/>
       <c r="E39" s="19"/>
-      <c r="F39" s="37"/>
-      <c r="G39" s="38"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="46"/>
       <c r="H39" s="8"/>
-      <c r="I39" s="41"/>
+      <c r="I39" s="38"/>
       <c r="J39" s="1"/>
     </row>
     <row r="40" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
-      <c r="C40" s="46"/>
-      <c r="D40" s="47"/>
+      <c r="C40" s="34"/>
+      <c r="D40" s="35"/>
       <c r="E40" s="19"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="38"/>
+      <c r="F40" s="45"/>
+      <c r="G40" s="46"/>
       <c r="H40" s="8"/>
-      <c r="I40" s="41"/>
+      <c r="I40" s="38"/>
       <c r="J40" s="1"/>
     </row>
     <row r="41" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
-      <c r="C41" s="46"/>
-      <c r="D41" s="47"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="35"/>
       <c r="E41" s="19"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="38"/>
+      <c r="F41" s="45"/>
+      <c r="G41" s="46"/>
       <c r="H41" s="8"/>
-      <c r="I41" s="41"/>
+      <c r="I41" s="38"/>
       <c r="J41" s="1"/>
     </row>
     <row r="42" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
-      <c r="C42" s="46"/>
-      <c r="D42" s="47"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="35"/>
       <c r="E42" s="19"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="38"/>
+      <c r="F42" s="45"/>
+      <c r="G42" s="46"/>
       <c r="H42" s="8"/>
-      <c r="I42" s="41"/>
+      <c r="I42" s="38"/>
       <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
-      <c r="C43" s="46"/>
-      <c r="D43" s="47"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="35"/>
       <c r="E43" s="19"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="38"/>
+      <c r="F43" s="45"/>
+      <c r="G43" s="46"/>
       <c r="H43" s="8"/>
-      <c r="I43" s="41"/>
+      <c r="I43" s="38"/>
       <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
-      <c r="C44" s="46"/>
-      <c r="D44" s="47"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="35"/>
       <c r="E44" s="19"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="38"/>
+      <c r="F44" s="45"/>
+      <c r="G44" s="46"/>
       <c r="H44" s="8"/>
-      <c r="I44" s="41"/>
+      <c r="I44" s="38"/>
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
-      <c r="C45" s="46"/>
-      <c r="D45" s="47"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="35"/>
       <c r="E45" s="19"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="38"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="46"/>
       <c r="H45" s="8"/>
-      <c r="I45" s="41"/>
+      <c r="I45" s="38"/>
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="47"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="35"/>
       <c r="E46" s="19"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="38"/>
+      <c r="F46" s="45"/>
+      <c r="G46" s="46"/>
       <c r="H46" s="8"/>
-      <c r="I46" s="41"/>
+      <c r="I46" s="38"/>
       <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
-      <c r="C47" s="46"/>
-      <c r="D47" s="47"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="35"/>
       <c r="E47" s="19"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="38"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="46"/>
       <c r="H47" s="8"/>
-      <c r="I47" s="41"/>
+      <c r="I47" s="38"/>
       <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
-      <c r="C48" s="46"/>
-      <c r="D48" s="47"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="35"/>
       <c r="E48" s="19"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="38"/>
+      <c r="F48" s="45"/>
+      <c r="G48" s="46"/>
       <c r="H48" s="8"/>
-      <c r="I48" s="41"/>
+      <c r="I48" s="38"/>
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
-      <c r="C49" s="46"/>
-      <c r="D49" s="47"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="35"/>
       <c r="E49" s="19"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="38"/>
+      <c r="F49" s="45"/>
+      <c r="G49" s="46"/>
       <c r="H49" s="8"/>
-      <c r="I49" s="41"/>
+      <c r="I49" s="38"/>
       <c r="J49" s="1"/>
     </row>
     <row r="50" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
-      <c r="C50" s="46"/>
-      <c r="D50" s="47"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="35"/>
       <c r="E50" s="19"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="38"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="46"/>
       <c r="H50" s="8"/>
-      <c r="I50" s="41"/>
+      <c r="I50" s="38"/>
       <c r="J50" s="1"/>
     </row>
     <row r="51" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
-      <c r="C51" s="46"/>
-      <c r="D51" s="47"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="35"/>
       <c r="E51" s="19"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="38"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="46"/>
       <c r="H51" s="8"/>
-      <c r="I51" s="41"/>
+      <c r="I51" s="38"/>
       <c r="J51" s="1"/>
     </row>
     <row r="52" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
-      <c r="C52" s="46"/>
-      <c r="D52" s="47"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="35"/>
       <c r="E52" s="19"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="38"/>
+      <c r="F52" s="45"/>
+      <c r="G52" s="46"/>
       <c r="H52" s="8"/>
-      <c r="I52" s="41"/>
+      <c r="I52" s="38"/>
       <c r="J52" s="1"/>
     </row>
     <row r="53" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
-      <c r="C53" s="46"/>
-      <c r="D53" s="47"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="35"/>
       <c r="E53" s="19"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="38"/>
+      <c r="F53" s="45"/>
+      <c r="G53" s="46"/>
       <c r="H53" s="8"/>
-      <c r="I53" s="41"/>
+      <c r="I53" s="38"/>
       <c r="J53" s="1"/>
     </row>
     <row r="54" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
-      <c r="C54" s="46"/>
-      <c r="D54" s="47"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="35"/>
       <c r="E54" s="19"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="38"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="46"/>
       <c r="H54" s="8"/>
-      <c r="I54" s="41"/>
+      <c r="I54" s="38"/>
       <c r="J54" s="1"/>
     </row>
     <row r="55" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
-      <c r="C55" s="46"/>
-      <c r="D55" s="47"/>
+      <c r="C55" s="34"/>
+      <c r="D55" s="35"/>
       <c r="E55" s="19"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="38"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="46"/>
       <c r="H55" s="8"/>
-      <c r="I55" s="41"/>
+      <c r="I55" s="38"/>
       <c r="J55" s="1"/>
     </row>
     <row r="56" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
-      <c r="C56" s="46"/>
-      <c r="D56" s="47"/>
+      <c r="C56" s="34"/>
+      <c r="D56" s="35"/>
       <c r="E56" s="19"/>
-      <c r="F56" s="37"/>
-      <c r="G56" s="38"/>
+      <c r="F56" s="45"/>
+      <c r="G56" s="46"/>
       <c r="H56" s="8"/>
-      <c r="I56" s="41"/>
+      <c r="I56" s="38"/>
       <c r="J56" s="1"/>
     </row>
     <row r="57" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
-      <c r="C57" s="46"/>
-      <c r="D57" s="47"/>
+      <c r="C57" s="34"/>
+      <c r="D57" s="35"/>
       <c r="E57" s="19"/>
-      <c r="F57" s="37"/>
-      <c r="G57" s="38"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="46"/>
       <c r="H57" s="8"/>
-      <c r="I57" s="41"/>
+      <c r="I57" s="38"/>
       <c r="J57" s="1"/>
     </row>
     <row r="58" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
-      <c r="C58" s="46"/>
-      <c r="D58" s="47"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="35"/>
       <c r="E58" s="19"/>
-      <c r="F58" s="37"/>
-      <c r="G58" s="38"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="46"/>
       <c r="H58" s="8"/>
-      <c r="I58" s="41"/>
+      <c r="I58" s="38"/>
       <c r="J58" s="1"/>
     </row>
     <row r="59" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
-      <c r="C59" s="46"/>
-      <c r="D59" s="47"/>
+      <c r="C59" s="34"/>
+      <c r="D59" s="35"/>
       <c r="E59" s="19"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="38"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="46"/>
       <c r="H59" s="8"/>
-      <c r="I59" s="41"/>
+      <c r="I59" s="38"/>
       <c r="J59" s="1"/>
     </row>
     <row r="60" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
-      <c r="C60" s="46"/>
-      <c r="D60" s="47"/>
+      <c r="C60" s="34"/>
+      <c r="D60" s="35"/>
       <c r="E60" s="19"/>
-      <c r="F60" s="37"/>
-      <c r="G60" s="38"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="46"/>
       <c r="H60" s="8"/>
-      <c r="I60" s="41"/>
+      <c r="I60" s="38"/>
       <c r="J60" s="1"/>
     </row>
     <row r="61" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
-      <c r="C61" s="46"/>
-      <c r="D61" s="47"/>
+      <c r="C61" s="34"/>
+      <c r="D61" s="35"/>
       <c r="E61" s="19"/>
-      <c r="F61" s="37"/>
-      <c r="G61" s="38"/>
+      <c r="F61" s="45"/>
+      <c r="G61" s="46"/>
       <c r="H61" s="8"/>
-      <c r="I61" s="41"/>
+      <c r="I61" s="38"/>
       <c r="J61" s="1"/>
     </row>
     <row r="62" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
-      <c r="C62" s="46"/>
-      <c r="D62" s="47"/>
+      <c r="C62" s="34"/>
+      <c r="D62" s="35"/>
       <c r="E62" s="19"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="38"/>
+      <c r="F62" s="45"/>
+      <c r="G62" s="46"/>
       <c r="H62" s="8"/>
-      <c r="I62" s="41"/>
+      <c r="I62" s="38"/>
       <c r="J62" s="1"/>
     </row>
     <row r="63" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
-      <c r="C63" s="46"/>
-      <c r="D63" s="47"/>
+      <c r="C63" s="34"/>
+      <c r="D63" s="35"/>
       <c r="E63" s="19"/>
-      <c r="F63" s="37"/>
-      <c r="G63" s="38"/>
+      <c r="F63" s="45"/>
+      <c r="G63" s="46"/>
       <c r="H63" s="8"/>
-      <c r="I63" s="41"/>
+      <c r="I63" s="38"/>
       <c r="J63" s="1"/>
     </row>
     <row r="64" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
-      <c r="C64" s="46"/>
-      <c r="D64" s="47"/>
+      <c r="C64" s="34"/>
+      <c r="D64" s="35"/>
       <c r="E64" s="19"/>
-      <c r="F64" s="37"/>
-      <c r="G64" s="38"/>
+      <c r="F64" s="45"/>
+      <c r="G64" s="46"/>
       <c r="H64" s="8"/>
-      <c r="I64" s="41"/>
+      <c r="I64" s="38"/>
       <c r="J64" s="1"/>
     </row>
     <row r="65" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
-      <c r="C65" s="46"/>
-      <c r="D65" s="47"/>
+      <c r="C65" s="34"/>
+      <c r="D65" s="35"/>
       <c r="E65" s="19"/>
-      <c r="F65" s="37"/>
-      <c r="G65" s="38"/>
+      <c r="F65" s="45"/>
+      <c r="G65" s="46"/>
       <c r="H65" s="8"/>
-      <c r="I65" s="41"/>
+      <c r="I65" s="38"/>
       <c r="J65" s="1"/>
     </row>
     <row r="66" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
-      <c r="C66" s="46"/>
-      <c r="D66" s="47"/>
+      <c r="C66" s="34"/>
+      <c r="D66" s="35"/>
       <c r="E66" s="19"/>
-      <c r="F66" s="37"/>
-      <c r="G66" s="38"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="46"/>
       <c r="H66" s="8"/>
-      <c r="I66" s="41"/>
+      <c r="I66" s="38"/>
       <c r="J66" s="1"/>
     </row>
     <row r="67" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
-      <c r="C67" s="46"/>
-      <c r="D67" s="47"/>
+      <c r="C67" s="34"/>
+      <c r="D67" s="35"/>
       <c r="E67" s="19"/>
-      <c r="F67" s="37"/>
-      <c r="G67" s="38"/>
+      <c r="F67" s="45"/>
+      <c r="G67" s="46"/>
       <c r="H67" s="8"/>
-      <c r="I67" s="41"/>
+      <c r="I67" s="38"/>
       <c r="J67" s="1"/>
     </row>
     <row r="68" spans="1:13" ht="47" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B68" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C68" s="48" t="s">
+      <c r="C68" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D68" s="48"/>
-      <c r="E68" s="49"/>
-      <c r="F68" s="34" t="s">
+      <c r="D68" s="36"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G68" s="34"/>
+      <c r="G68" s="47"/>
       <c r="H68" s="28">
         <f>SUM(H8:H67)</f>
         <v>0</v>
@@ -1708,8 +1708,8 @@
     <row r="70" spans="1:13" ht="26" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="17"/>
       <c r="B70" s="17"/>
-      <c r="C70" s="35"/>
-      <c r="D70" s="35"/>
+      <c r="C70" s="48"/>
+      <c r="D70" s="48"/>
       <c r="E70" s="18"/>
       <c r="F70" s="18"/>
       <c r="G70" s="18"/>
@@ -1755,50 +1755,69 @@
     </row>
   </sheetData>
   <mergeCells count="131">
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="F68:G68"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="F64:G64"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="F56:G56"/>
+    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F59:G59"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="F53:G53"/>
+    <mergeCell ref="F54:G54"/>
+    <mergeCell ref="F55:G55"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="I8:I67"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E2:F2"/>
@@ -1823,69 +1842,50 @@
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="F68:G68"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="F64:G64"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="F56:G56"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F59:G59"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="F53:G53"/>
-    <mergeCell ref="F54:G54"/>
-    <mergeCell ref="F55:G55"/>
-    <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C37:D37"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="C60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0" right="0" top="0.1" bottom="0" header="0" footer="0.1"/>

</xml_diff>